<commit_message>
Added the callbacks for the dropdown
</commit_message>
<xml_diff>
--- a/data/lab4_drug-description.xlsx
+++ b/data/lab4_drug-description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apitt\Documents\UBC\MDS\532_DS_viz2\DSCI_532_Group_113_Overdose\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4EACD76D-719D-46D8-B0AC-56ED6BC8FF12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D80CE25-41B1-4398-9591-8D4E8225C27F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2200C2C8-EF8B-4EAE-95C9-AE9F1803E73F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Drug</t>
   </si>
@@ -478,6 +478,15 @@
   </si>
   <si>
     <t>https://www.drugbank.ca/drugs/DB00813</t>
+  </si>
+  <si>
+    <t>Everything</t>
+  </si>
+  <si>
+    <t>No drug selected</t>
+  </si>
+  <si>
+    <t>https://www.drugbank.ca/assets/logo-pink-bd7264e3b993f48d681445728e394507ac912eb6e426e52c6d3230a78dae4bc6.svg</t>
   </si>
 </sst>
 </file>
@@ -865,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{957C0A05-3243-4389-AFB0-D9459F1B2568}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1067,6 +1076,17 @@
       </c>
       <c r="D14" s="3" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>